<commit_message>
change table names in the cube to have fact and dim prefixes
</commit_message>
<xml_diff>
--- a/Reports/PaymentUseCase_001.xlsx
+++ b/Reports/PaymentUseCase_001.xlsx
@@ -17,16 +17,17 @@
   <definedNames>
     <definedName name="Slicer_Day">#N/A</definedName>
     <definedName name="Slicer_MonthName">#N/A</definedName>
+    <definedName name="Slicer_PaymentUseCases">#N/A</definedName>
     <definedName name="Slicer_YearNumber">#N/A</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="97" r:id="rId2"/>
+    <pivotCache cacheId="82" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{876F7934-8845-4945-9796-88D515C7AA90}">
       <x14:pivotCaches>
-        <pivotCache cacheId="88" r:id="rId3"/>
+        <pivotCache cacheId="67" r:id="rId3"/>
       </x14:pivotCaches>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -34,6 +35,7 @@
         <x14:slicerCache r:id="rId4"/>
         <x14:slicerCache r:id="rId5"/>
         <x14:slicerCache r:id="rId6"/>
+        <x14:slicerCache r:id="rId7"/>
       </x14:slicerCaches>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -56,18 +58,156 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="50">
   <si>
     <t>Row Labels</t>
   </si>
   <si>
-    <t>Cash-In | Cash-Out</t>
-  </si>
-  <si>
-    <t>Cash-Out By Customer</t>
-  </si>
-  <si>
-    <t>Cash-Out By Unregistered</t>
+    <t>BaseTransaction</t>
+  </si>
+  <si>
+    <t>TxCount</t>
+  </si>
+  <si>
+    <t>Electronic Non-Personal Payments within MMO</t>
+  </si>
+  <si>
+    <t>B2P Bulk Batched Payments into Accounts</t>
+  </si>
+  <si>
+    <t>B2P Bulk Batched Payments to Unregistered</t>
+  </si>
+  <si>
+    <t>G2P Bulk Batched Payments into Accounts</t>
+  </si>
+  <si>
+    <t>G2P Bulk Batched Payments to Unregistered</t>
+  </si>
+  <si>
+    <t>AGENT_ACCEPT_DEPOSIT</t>
+  </si>
+  <si>
+    <t>AGENT_ACCEPT_DEPOSIT_COMMISSION</t>
+  </si>
+  <si>
+    <t>AGENT_BFS_ACCEPT_DEPOSIT</t>
+  </si>
+  <si>
+    <t>AGENT_BFS_ACCEPT_WITHDRAWAL</t>
+  </si>
+  <si>
+    <t>AGENT_BFS_COMMISSION</t>
+  </si>
+  <si>
+    <t>AGENT_BILL_PAY</t>
+  </si>
+  <si>
+    <t>AGENT_BILL_PAY_FROM_STOCK</t>
+  </si>
+  <si>
+    <t>AGENT_DEPOSIT_TO_BANK_ACCOUNT</t>
+  </si>
+  <si>
+    <t>AGENT_DISPENSE_CASH_FOR_SEND_CASH</t>
+  </si>
+  <si>
+    <t>AGENT_DISPENSE_CASH_FOR_WITHDRAWAL</t>
+  </si>
+  <si>
+    <t>AGENT_SELL_AIRTIME_PRE_PAID</t>
+  </si>
+  <si>
+    <t>AGENT_SEND_CASH_CUSTOMER_TO_CUSTOMER</t>
+  </si>
+  <si>
+    <t>AGENT_SEND_CASH_CUSTOMER_TO_NONCUSTOMER</t>
+  </si>
+  <si>
+    <t>AGENT_SIGN_UP_CUSTOMER</t>
+  </si>
+  <si>
+    <t>AGENT_SIGN_UP_CUSTOMER_COMMISSION</t>
+  </si>
+  <si>
+    <t>BULK_PAY_AIRTIME_DISCOUNT_AWARD</t>
+  </si>
+  <si>
+    <t>BULK_PAY_BUY_AIRTIME_PRE_PAID</t>
+  </si>
+  <si>
+    <t>BULK_PAY_SEND_CASH_TO_CUSTOMER</t>
+  </si>
+  <si>
+    <t>CUSTOMER_BILL_PAY</t>
+  </si>
+  <si>
+    <t>CUSTOMER_BILL_PAY_FROM_STOCK</t>
+  </si>
+  <si>
+    <t>CUSTOMER_BUY_AIRTIME_PRE_PAID</t>
+  </si>
+  <si>
+    <t>CUSTOMER_REQUEST_WITHDRAW_CASH</t>
+  </si>
+  <si>
+    <t>CUSTOMER_SEND_CASH_TO_CUSTOMER</t>
+  </si>
+  <si>
+    <t>CUSTOMER_SEND_CASH_TO_NON_CUSTOMER_UNCLAIMED</t>
+  </si>
+  <si>
+    <t>CUSTOMER_SEND_CASH_TO_NONCUSTOMER</t>
+  </si>
+  <si>
+    <t>GENERIC_MIRRORING_REFUND_TRANSACTION_TYPE</t>
+  </si>
+  <si>
+    <t>ORGANIZATION_WITHDRAWAL_MANUAL</t>
+  </si>
+  <si>
+    <t>PAGA_BFS_SETTLEMENT</t>
+  </si>
+  <si>
+    <t>PAGA_COLLECT_THIRD_PARTY_RECEIVABLES</t>
+  </si>
+  <si>
+    <t>PAGA_HOLD_ACCOUNT_BALANCE</t>
+  </si>
+  <si>
+    <t>PAGA_PAY_BANK_WITHDRAW_TO_BANK_ACCOUNT_COMMISSION</t>
+  </si>
+  <si>
+    <t>PAGA_PAY_THIRD_PARTY_PAYABLE</t>
+  </si>
+  <si>
+    <t>PAGA_POOL_ACCOUNT_TRANSFER</t>
+  </si>
+  <si>
+    <t>PAGA_UNHOLD_ACCOUNT_BALANCE</t>
+  </si>
+  <si>
+    <t>USER_BILL_PAY_REFUND</t>
+  </si>
+  <si>
+    <t>USER_DEPOSIT_FROM_BANK_ACCOUNT</t>
+  </si>
+  <si>
+    <t>USER_DEPOSIT_FROM_CARD</t>
+  </si>
+  <si>
+    <t>USER_DEPOSIT_FROM_CARD_FREE</t>
+  </si>
+  <si>
+    <t>USER_PREMIUM_SMS</t>
+  </si>
+  <si>
+    <t>USER_REMITTANCE_COLLECTION</t>
+  </si>
+  <si>
+    <t>USER_SEND_CASH_TO_BANK_ACCOUNT</t>
+  </si>
+  <si>
+    <t>USER_TRANSFER_FROM_CASH_BONUS_ACCOUNT</t>
   </si>
 </sst>
 </file>
@@ -103,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -112,42 +252,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -183,13 +297,13 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="0" y="114300"/>
-          <a:ext cx="4448175" cy="2524125"/>
+          <a:ext cx="6715125" cy="2524125"/>
           <a:chOff x="5791200" y="2943225"/>
           <a:chExt cx="5638800" cy="2524125"/>
         </a:xfrm>
       </xdr:grpSpPr>
-      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-        <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+        <mc:Choice Requires="a14">
           <xdr:graphicFrame macro="">
             <xdr:nvGraphicFramePr>
               <xdr:cNvPr id="7" name="YearNumber"/>
@@ -206,7 +320,7 @@
             </a:graphic>
           </xdr:graphicFrame>
         </mc:Choice>
-        <mc:Fallback>
+        <mc:Fallback xmlns="">
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
               <xdr:cNvPr id="0" name=""/>
@@ -245,8 +359,8 @@
           </xdr:sp>
         </mc:Fallback>
       </mc:AlternateContent>
-      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-        <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+        <mc:Choice Requires="a14">
           <xdr:graphicFrame macro="">
             <xdr:nvGraphicFramePr>
               <xdr:cNvPr id="8" name="MonthName"/>
@@ -263,7 +377,7 @@
             </a:graphic>
           </xdr:graphicFrame>
         </mc:Choice>
-        <mc:Fallback>
+        <mc:Fallback xmlns="">
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
               <xdr:cNvPr id="0" name=""/>
@@ -302,8 +416,8 @@
           </xdr:sp>
         </mc:Fallback>
       </mc:AlternateContent>
-      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-        <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+        <mc:Choice Requires="a14">
           <xdr:graphicFrame macro="">
             <xdr:nvGraphicFramePr>
               <xdr:cNvPr id="9" name="Day"/>
@@ -320,7 +434,7 @@
             </a:graphic>
           </xdr:graphicFrame>
         </mc:Choice>
-        <mc:Fallback>
+        <mc:Fallback xmlns="">
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
               <xdr:cNvPr id="0" name=""/>
@@ -362,13 +476,85 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="PaymentUseCaseType"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="PaymentUseCaseType"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8220075" y="942975"/>
+              <a:ext cx="1828800" cy="3990975"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Christina Leo" refreshedDate="42069.541834606483" backgroundQuery="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Christina Leo" refreshedDate="42069.648598958331" backgroundQuery="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
   <cacheSource type="external" connectionId="1"/>
-  <cacheFields count="10">
+  <cacheFields count="13">
     <cacheField name="[FinancialTransaction].[Cancelled].[Cancelled]" caption="Cancelled" numFmtId="0" hierarchy="2" level="1">
       <sharedItems count="1">
         <s v="[FinancialTransaction].[Cancelled].&amp;[1]" c="1"/>
@@ -385,13 +571,15 @@
     </cacheField>
     <cacheField name="[PaymentUseCase].[PaymentUseCases].[PaymentUseCaseType]" caption="PaymentUseCaseType" numFmtId="0" hierarchy="120" level="1">
       <sharedItems count="1">
-        <s v="[PaymentUseCase].[PaymentUseCases].[PaymentUseCaseType].&amp;[Cash-In | Cash-Out]" c="Cash-In | Cash-Out"/>
+        <s v="[PaymentUseCase].[PaymentUseCases].[PaymentUseCaseType].&amp;[Electronic Non-Personal Payments within MMO]" c="Electronic Non-Personal Payments within MMO"/>
       </sharedItems>
     </cacheField>
     <cacheField name="[PaymentUseCase].[PaymentUseCases].[PaymentUseCase]" caption="PaymentUseCase" numFmtId="0" hierarchy="120" level="2">
-      <sharedItems count="2">
-        <s v="[PaymentUseCase].[PaymentUseCases].[PaymentUseCase].&amp;[Cash-Out By Customer]" c="Cash-Out By Customer"/>
-        <s v="[PaymentUseCase].[PaymentUseCases].[PaymentUseCase].&amp;[Cash-Out By Unregistered]" c="Cash-Out By Unregistered"/>
+      <sharedItems count="4">
+        <s v="[PaymentUseCase].[PaymentUseCases].[PaymentUseCase].&amp;[B2P Bulk Batched Payments into Accounts]" c="B2P Bulk Batched Payments into Accounts"/>
+        <s v="[PaymentUseCase].[PaymentUseCases].[PaymentUseCase].&amp;[B2P Bulk Batched Payments to Unregistered]" c="B2P Bulk Batched Payments to Unregistered"/>
+        <s v="[PaymentUseCase].[PaymentUseCases].[PaymentUseCase].&amp;[G2P Bulk Batched Payments into Accounts]" c="G2P Bulk Batched Payments into Accounts"/>
+        <s v="[PaymentUseCase].[PaymentUseCases].[PaymentUseCase].&amp;[G2P Bulk Batched Payments to Unregistered]" c="G2P Bulk Batched Payments to Unregistered"/>
       </sharedItems>
     </cacheField>
     <cacheField name="[ProcessCompletedDate].[YearNumber].[YearNumber]" caption="YearNumber" numFmtId="0" hierarchy="151" level="1">
@@ -405,6 +593,54 @@
     </cacheField>
     <cacheField name="[TransactionDate].[Day].[Day]" caption="Day" numFmtId="0" hierarchy="239" level="1">
       <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+    <cacheField name="[Measures].[BaseTransaction]" caption="BaseTransaction" numFmtId="0" hierarchy="300" level="32767"/>
+    <cacheField name="[Measures].[TxCount]" caption="TxCount" numFmtId="0" hierarchy="295" level="32767"/>
+    <cacheField name="[FinancialTransactionType].[FinancialTransactionType].[FinancialTransactionType]" caption="FinancialTransactionType" numFmtId="0" hierarchy="26" level="1">
+      <sharedItems count="42">
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_ACCEPT_DEPOSIT]" c="AGENT_ACCEPT_DEPOSIT"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_ACCEPT_DEPOSIT_COMMISSION]" c="AGENT_ACCEPT_DEPOSIT_COMMISSION"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_BFS_ACCEPT_DEPOSIT]" c="AGENT_BFS_ACCEPT_DEPOSIT"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_BFS_ACCEPT_WITHDRAWAL]" c="AGENT_BFS_ACCEPT_WITHDRAWAL"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_BFS_COMMISSION]" c="AGENT_BFS_COMMISSION"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_BILL_PAY]" c="AGENT_BILL_PAY"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_BILL_PAY_FROM_STOCK]" c="AGENT_BILL_PAY_FROM_STOCK"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_DEPOSIT_TO_BANK_ACCOUNT]" c="AGENT_DEPOSIT_TO_BANK_ACCOUNT"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_DISPENSE_CASH_FOR_SEND_CASH]" c="AGENT_DISPENSE_CASH_FOR_SEND_CASH"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_DISPENSE_CASH_FOR_WITHDRAWAL]" c="AGENT_DISPENSE_CASH_FOR_WITHDRAWAL"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_SELL_AIRTIME_PRE_PAID]" c="AGENT_SELL_AIRTIME_PRE_PAID"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_SEND_CASH_CUSTOMER_TO_CUSTOMER]" c="AGENT_SEND_CASH_CUSTOMER_TO_CUSTOMER"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_SEND_CASH_CUSTOMER_TO_NONCUSTOMER]" c="AGENT_SEND_CASH_CUSTOMER_TO_NONCUSTOMER"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_SIGN_UP_CUSTOMER]" c="AGENT_SIGN_UP_CUSTOMER"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[AGENT_SIGN_UP_CUSTOMER_COMMISSION]" c="AGENT_SIGN_UP_CUSTOMER_COMMISSION"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[BULK_PAY_AIRTIME_DISCOUNT_AWARD]" c="BULK_PAY_AIRTIME_DISCOUNT_AWARD"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[BULK_PAY_BUY_AIRTIME_PRE_PAID]" c="BULK_PAY_BUY_AIRTIME_PRE_PAID"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[BULK_PAY_SEND_CASH_TO_CUSTOMER]" c="BULK_PAY_SEND_CASH_TO_CUSTOMER"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[CUSTOMER_BILL_PAY]" c="CUSTOMER_BILL_PAY"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[CUSTOMER_BILL_PAY_FROM_STOCK]" c="CUSTOMER_BILL_PAY_FROM_STOCK"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[CUSTOMER_BUY_AIRTIME_PRE_PAID]" c="CUSTOMER_BUY_AIRTIME_PRE_PAID"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[CUSTOMER_REQUEST_WITHDRAW_CASH]" c="CUSTOMER_REQUEST_WITHDRAW_CASH"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[CUSTOMER_SEND_CASH_TO_CUSTOMER]" c="CUSTOMER_SEND_CASH_TO_CUSTOMER"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[CUSTOMER_SEND_CASH_TO_NON_CUSTOMER_UNCLAIMED]" c="CUSTOMER_SEND_CASH_TO_NON_CUSTOMER_UNCLAIMED"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[CUSTOMER_SEND_CASH_TO_NONCUSTOMER]" c="CUSTOMER_SEND_CASH_TO_NONCUSTOMER"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[GENERIC_MIRRORING_REFUND_TRANSACTION_TYPE]" c="GENERIC_MIRRORING_REFUND_TRANSACTION_TYPE"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[ORGANIZATION_WITHDRAWAL_MANUAL]" c="ORGANIZATION_WITHDRAWAL_MANUAL"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[PAGA_BFS_SETTLEMENT]" c="PAGA_BFS_SETTLEMENT"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[PAGA_COLLECT_THIRD_PARTY_RECEIVABLES]" c="PAGA_COLLECT_THIRD_PARTY_RECEIVABLES"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[PAGA_HOLD_ACCOUNT_BALANCE]" c="PAGA_HOLD_ACCOUNT_BALANCE"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[PAGA_PAY_BANK_WITHDRAW_TO_BANK_ACCOUNT_COMMISSION]" c="PAGA_PAY_BANK_WITHDRAW_TO_BANK_ACCOUNT_COMMISSION"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[PAGA_PAY_THIRD_PARTY_PAYABLE]" c="PAGA_PAY_THIRD_PARTY_PAYABLE"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[PAGA_POOL_ACCOUNT_TRANSFER]" c="PAGA_POOL_ACCOUNT_TRANSFER"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[PAGA_UNHOLD_ACCOUNT_BALANCE]" c="PAGA_UNHOLD_ACCOUNT_BALANCE"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[USER_BILL_PAY_REFUND]" c="USER_BILL_PAY_REFUND"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[USER_DEPOSIT_FROM_BANK_ACCOUNT]" c="USER_DEPOSIT_FROM_BANK_ACCOUNT"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[USER_DEPOSIT_FROM_CARD]" c="USER_DEPOSIT_FROM_CARD"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[USER_DEPOSIT_FROM_CARD_FREE]" c="USER_DEPOSIT_FROM_CARD_FREE"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[USER_PREMIUM_SMS]" c="USER_PREMIUM_SMS"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[USER_REMITTANCE_COLLECTION]" c="USER_REMITTANCE_COLLECTION"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[USER_SEND_CASH_TO_BANK_ACCOUNT]" c="USER_SEND_CASH_TO_BANK_ACCOUNT"/>
+        <s v="[FinancialTransactionType].[FinancialTransactionType].&amp;[USER_TRANSFER_FROM_CASH_BONUS_ACCOUNT]" c="USER_TRANSFER_FROM_CASH_BONUS_ACCOUNT"/>
+      </sharedItems>
     </cacheField>
   </cacheFields>
   <cacheHierarchies count="330">
@@ -439,7 +675,12 @@
     <cacheHierarchy uniqueName="[FinancialTransaction].[ShortCode]" caption="ShortCode" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[ShortCode].[All]" allUniqueName="[FinancialTransaction].[ShortCode].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[FinancialTransaction].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[SourceKey].[All]" allUniqueName="[FinancialTransaction].[SourceKey].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="2" unbalanced="0"/>
     <cacheHierarchy uniqueName="[FinancialTransaction].[TextDescription]" caption="TextDescription" attribute="1" defaultMemberUniqueName="[FinancialTransaction].[TextDescription].[All]" allUniqueName="[FinancialTransaction].[TextDescription].[All]" dimensionUniqueName="[FinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[FinancialTransactionType].[FinancialTransactionType]" caption="FinancialTransactionType" attribute="1" defaultMemberUniqueName="[FinancialTransactionType].[FinancialTransactionType].[All]" allUniqueName="[FinancialTransactionType].[FinancialTransactionType].[All]" dimensionUniqueName="[FinancialTransactionType]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[FinancialTransactionType].[FinancialTransactionType]" caption="FinancialTransactionType" attribute="1" defaultMemberUniqueName="[FinancialTransactionType].[FinancialTransactionType].[All]" allUniqueName="[FinancialTransactionType].[FinancialTransactionType].[All]" dimensionUniqueName="[FinancialTransactionType]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="12"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[ForUser].[DimCreatedDateID]" caption="DimCreatedDateID" attribute="1" defaultMemberUniqueName="[ForUser].[DimCreatedDateID].[All]" allUniqueName="[ForUser].[DimCreatedDateID].[All]" dimensionUniqueName="[ForUser]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[ForUser].[DimDateOfBirthID]" caption="DimDateOfBirthID" attribute="1" defaultMemberUniqueName="[ForUser].[DimDateOfBirthID].[All]" allUniqueName="[ForUser].[DimDateOfBirthID].[All]" dimensionUniqueName="[ForUser]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[ForUser].[DimForUserID]" caption="DimForUserID" attribute="1" defaultMemberUniqueName="[ForUser].[DimForUserID].[All]" allUniqueName="[ForUser].[DimForUserID].[All]" dimensionUniqueName="[ForUser]" displayFolder="" count="0" unbalanced="0"/>
@@ -749,12 +990,20 @@
     <cacheHierarchy uniqueName="[PaymentUseCase].[DimFinancialTxTypeID]" caption="DimFinancialTxTypeID" attribute="1" defaultMemberUniqueName="[PaymentUseCase].[DimFinancialTxTypeID].[All]" allUniqueName="[PaymentUseCase].[DimFinancialTxTypeID].[All]" dimensionUniqueName="[PaymentUseCase]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
     <cacheHierarchy uniqueName="[PaymentUseCase].[PaymentUseCase]" caption="PaymentUseCase" attribute="1" defaultMemberUniqueName="[PaymentUseCase].[PaymentUseCase].[All]" allUniqueName="[PaymentUseCase].[PaymentUseCase].[All]" dimensionUniqueName="[PaymentUseCase]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
     <cacheHierarchy uniqueName="[PaymentUseCase].[PaymentUseCaseType]" caption="PaymentUseCaseType" attribute="1" defaultMemberUniqueName="[PaymentUseCase].[PaymentUseCaseType].[All]" allUniqueName="[PaymentUseCase].[PaymentUseCaseType].[All]" dimensionUniqueName="[PaymentUseCase]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[TxCount]" caption="TxCount" measure="1" displayFolder="" measureGroup="GLTransaction" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[TxCount]" caption="TxCount" measure="1" displayFolder="" measureGroup="GLTransaction" count="0" oneField="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="11"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[Measures].[Credits]" caption="Credits" measure="1" displayFolder="" measureGroup="GLTransaction" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Debits]" caption="Debits" measure="1" displayFolder="" measureGroup="GLTransaction" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Balance]" caption="Balance" measure="1" displayFolder="" measureGroup="GLTransaction" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[ProcessEventCount]" caption="ProcessEventCount" measure="1" displayFolder="" measureGroup="ProcessEvent" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[BaseTransaction]" caption="BaseTransaction" measure="1" displayFolder="" measureGroup="FinancialTransaction" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[BaseTransaction]" caption="BaseTransaction" measure="1" displayFolder="" measureGroup="FinancialTransaction" count="0" oneField="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="10"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[Measures].[TxAmount]" caption="TxAmount" measure="1" displayFolder="" measureGroup="GLTransaction" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[ProcessTxAmt]" caption="ProcessTxAmt" measure="1" displayFolder="" measureGroup="ProcessEvent" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[LineItemCount]" caption="LineItemCount" measure="1" displayFolder="" measureGroup="GLTransaction" count="0"/>
@@ -1040,7 +1289,7 @@
     <cacheHierarchy uniqueName="[PagaAccountUserType].[DimPagaAccountUserTypeID]" caption="DimPagaAccountUserTypeID" attribute="1" defaultMemberUniqueName="[PagaAccountUserType].[DimPagaAccountUserTypeID].[All]" allUniqueName="[PagaAccountUserType].[DimPagaAccountUserTypeID].[All]" dimensionUniqueName="[PagaAccountUserType]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[PagaAccountUserType].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[PagaAccountUserType].[Name].[All]" allUniqueName="[PagaAccountUserType].[Name].[All]" dimensionUniqueName="[PagaAccountUserType]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[PagaAccountUserType].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[PagaAccountUserType].[SourceKey].[All]" allUniqueName="[PagaAccountUserType].[SourceKey].[All]" dimensionUniqueName="[PagaAccountUserType]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[PaymentUseCase].[PaymentUseCases]" caption="PaymentUseCases" defaultMemberUniqueName="[PaymentUseCase].[PaymentUseCases].[All]" allUniqueName="[PaymentUseCase].[PaymentUseCases].[All]" dimensionUniqueName="[PaymentUseCase]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[PaymentUseCase].[PaymentUseCases]" caption="PaymentUseCases" defaultMemberUniqueName="[PaymentUseCase].[PaymentUseCases].[All]" allUniqueName="[PaymentUseCase].[PaymentUseCases].[All]" dimensionUniqueName="[PaymentUseCase]" displayFolder="" count="3" unbalanced="0"/>
     <cacheHierarchy uniqueName="[ProcessChannel].[DimProcessChannelID]" caption="DimProcessChannelID" attribute="1" defaultMemberUniqueName="[ProcessChannel].[DimProcessChannelID].[All]" allUniqueName="[ProcessChannel].[DimProcessChannelID].[All]" dimensionUniqueName="[ProcessChannel]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[ProcessChannel].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[ProcessChannel].[Name].[All]" allUniqueName="[ProcessChannel].[Name].[All]" dimensionUniqueName="[ProcessChannel]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[ProcessChannel].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[ProcessChannel].[SourceKey].[All]" allUniqueName="[ProcessChannel].[SourceKey].[All]" dimensionUniqueName="[ProcessChannel]" displayFolder="" count="0" unbalanced="0"/>
@@ -1261,9 +1510,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="97" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" colHeaderCaption="Has Financia lTransaction" fieldListSortAscending="1">
-  <location ref="A16:A19" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="10">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="82" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" colHeaderCaption="Has Financia lTransaction" fieldListSortAscending="1">
+  <location ref="A16:C189" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="13">
     <pivotField allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
       <items count="2">
         <item s="1" x="0"/>
@@ -1275,14 +1524,16 @@
     <pivotField allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1"/>
     <pivotField axis="axisRow" allDrilled="1" showAll="0" dataSourceSort="1">
       <items count="2">
-        <item s="1" c="1" x="0" d="1"/>
+        <item s="1" c="1" x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" showAll="0" dataSourceSort="1">
-      <items count="3">
+    <pivotField axis="axisRow" allDrilled="1" showAll="0" dataSourceSort="1">
+      <items count="5">
         <item x="0"/>
         <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1290,22 +1541,597 @@
     <pivotField allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1"/>
     <pivotField allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1"/>
     <pivotField allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
+      <items count="43">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
   </pivotFields>
-  <rowFields count="2">
+  <rowFields count="3">
     <field x="4"/>
     <field x="5"/>
+    <field x="12"/>
   </rowFields>
-  <rowItems count="3">
+  <rowItems count="173">
     <i>
       <x/>
     </i>
     <i r="1">
       <x/>
     </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="4"/>
+    </i>
+    <i r="2">
+      <x v="5"/>
+    </i>
+    <i r="2">
+      <x v="6"/>
+    </i>
+    <i r="2">
+      <x v="7"/>
+    </i>
+    <i r="2">
+      <x v="8"/>
+    </i>
+    <i r="2">
+      <x v="9"/>
+    </i>
+    <i r="2">
+      <x v="10"/>
+    </i>
+    <i r="2">
+      <x v="11"/>
+    </i>
+    <i r="2">
+      <x v="12"/>
+    </i>
+    <i r="2">
+      <x v="13"/>
+    </i>
+    <i r="2">
+      <x v="14"/>
+    </i>
+    <i r="2">
+      <x v="15"/>
+    </i>
+    <i r="2">
+      <x v="16"/>
+    </i>
+    <i r="2">
+      <x v="17"/>
+    </i>
+    <i r="2">
+      <x v="18"/>
+    </i>
+    <i r="2">
+      <x v="19"/>
+    </i>
+    <i r="2">
+      <x v="20"/>
+    </i>
+    <i r="2">
+      <x v="21"/>
+    </i>
+    <i r="2">
+      <x v="22"/>
+    </i>
+    <i r="2">
+      <x v="23"/>
+    </i>
+    <i r="2">
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="25"/>
+    </i>
+    <i r="2">
+      <x v="26"/>
+    </i>
+    <i r="2">
+      <x v="27"/>
+    </i>
+    <i r="2">
+      <x v="28"/>
+    </i>
+    <i r="2">
+      <x v="29"/>
+    </i>
+    <i r="2">
+      <x v="30"/>
+    </i>
+    <i r="2">
+      <x v="31"/>
+    </i>
+    <i r="2">
+      <x v="32"/>
+    </i>
+    <i r="2">
+      <x v="33"/>
+    </i>
+    <i r="2">
+      <x v="34"/>
+    </i>
+    <i r="2">
+      <x v="35"/>
+    </i>
+    <i r="2">
+      <x v="36"/>
+    </i>
+    <i r="2">
+      <x v="37"/>
+    </i>
+    <i r="2">
+      <x v="38"/>
+    </i>
+    <i r="2">
+      <x v="39"/>
+    </i>
+    <i r="2">
+      <x v="40"/>
+    </i>
+    <i r="2">
+      <x v="41"/>
+    </i>
     <i r="1">
       <x v="1"/>
     </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="4"/>
+    </i>
+    <i r="2">
+      <x v="5"/>
+    </i>
+    <i r="2">
+      <x v="6"/>
+    </i>
+    <i r="2">
+      <x v="7"/>
+    </i>
+    <i r="2">
+      <x v="8"/>
+    </i>
+    <i r="2">
+      <x v="9"/>
+    </i>
+    <i r="2">
+      <x v="10"/>
+    </i>
+    <i r="2">
+      <x v="11"/>
+    </i>
+    <i r="2">
+      <x v="12"/>
+    </i>
+    <i r="2">
+      <x v="13"/>
+    </i>
+    <i r="2">
+      <x v="14"/>
+    </i>
+    <i r="2">
+      <x v="15"/>
+    </i>
+    <i r="2">
+      <x v="16"/>
+    </i>
+    <i r="2">
+      <x v="17"/>
+    </i>
+    <i r="2">
+      <x v="18"/>
+    </i>
+    <i r="2">
+      <x v="19"/>
+    </i>
+    <i r="2">
+      <x v="20"/>
+    </i>
+    <i r="2">
+      <x v="21"/>
+    </i>
+    <i r="2">
+      <x v="22"/>
+    </i>
+    <i r="2">
+      <x v="23"/>
+    </i>
+    <i r="2">
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="25"/>
+    </i>
+    <i r="2">
+      <x v="26"/>
+    </i>
+    <i r="2">
+      <x v="27"/>
+    </i>
+    <i r="2">
+      <x v="28"/>
+    </i>
+    <i r="2">
+      <x v="29"/>
+    </i>
+    <i r="2">
+      <x v="30"/>
+    </i>
+    <i r="2">
+      <x v="31"/>
+    </i>
+    <i r="2">
+      <x v="32"/>
+    </i>
+    <i r="2">
+      <x v="33"/>
+    </i>
+    <i r="2">
+      <x v="34"/>
+    </i>
+    <i r="2">
+      <x v="35"/>
+    </i>
+    <i r="2">
+      <x v="36"/>
+    </i>
+    <i r="2">
+      <x v="37"/>
+    </i>
+    <i r="2">
+      <x v="38"/>
+    </i>
+    <i r="2">
+      <x v="39"/>
+    </i>
+    <i r="2">
+      <x v="40"/>
+    </i>
+    <i r="2">
+      <x v="41"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="4"/>
+    </i>
+    <i r="2">
+      <x v="5"/>
+    </i>
+    <i r="2">
+      <x v="6"/>
+    </i>
+    <i r="2">
+      <x v="7"/>
+    </i>
+    <i r="2">
+      <x v="8"/>
+    </i>
+    <i r="2">
+      <x v="9"/>
+    </i>
+    <i r="2">
+      <x v="10"/>
+    </i>
+    <i r="2">
+      <x v="11"/>
+    </i>
+    <i r="2">
+      <x v="12"/>
+    </i>
+    <i r="2">
+      <x v="13"/>
+    </i>
+    <i r="2">
+      <x v="14"/>
+    </i>
+    <i r="2">
+      <x v="15"/>
+    </i>
+    <i r="2">
+      <x v="16"/>
+    </i>
+    <i r="2">
+      <x v="17"/>
+    </i>
+    <i r="2">
+      <x v="18"/>
+    </i>
+    <i r="2">
+      <x v="19"/>
+    </i>
+    <i r="2">
+      <x v="20"/>
+    </i>
+    <i r="2">
+      <x v="21"/>
+    </i>
+    <i r="2">
+      <x v="22"/>
+    </i>
+    <i r="2">
+      <x v="23"/>
+    </i>
+    <i r="2">
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="25"/>
+    </i>
+    <i r="2">
+      <x v="26"/>
+    </i>
+    <i r="2">
+      <x v="27"/>
+    </i>
+    <i r="2">
+      <x v="28"/>
+    </i>
+    <i r="2">
+      <x v="29"/>
+    </i>
+    <i r="2">
+      <x v="30"/>
+    </i>
+    <i r="2">
+      <x v="31"/>
+    </i>
+    <i r="2">
+      <x v="32"/>
+    </i>
+    <i r="2">
+      <x v="33"/>
+    </i>
+    <i r="2">
+      <x v="34"/>
+    </i>
+    <i r="2">
+      <x v="35"/>
+    </i>
+    <i r="2">
+      <x v="36"/>
+    </i>
+    <i r="2">
+      <x v="37"/>
+    </i>
+    <i r="2">
+      <x v="38"/>
+    </i>
+    <i r="2">
+      <x v="39"/>
+    </i>
+    <i r="2">
+      <x v="40"/>
+    </i>
+    <i r="2">
+      <x v="41"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="4"/>
+    </i>
+    <i r="2">
+      <x v="5"/>
+    </i>
+    <i r="2">
+      <x v="6"/>
+    </i>
+    <i r="2">
+      <x v="7"/>
+    </i>
+    <i r="2">
+      <x v="8"/>
+    </i>
+    <i r="2">
+      <x v="9"/>
+    </i>
+    <i r="2">
+      <x v="10"/>
+    </i>
+    <i r="2">
+      <x v="11"/>
+    </i>
+    <i r="2">
+      <x v="12"/>
+    </i>
+    <i r="2">
+      <x v="13"/>
+    </i>
+    <i r="2">
+      <x v="14"/>
+    </i>
+    <i r="2">
+      <x v="15"/>
+    </i>
+    <i r="2">
+      <x v="16"/>
+    </i>
+    <i r="2">
+      <x v="17"/>
+    </i>
+    <i r="2">
+      <x v="18"/>
+    </i>
+    <i r="2">
+      <x v="19"/>
+    </i>
+    <i r="2">
+      <x v="20"/>
+    </i>
+    <i r="2">
+      <x v="21"/>
+    </i>
+    <i r="2">
+      <x v="22"/>
+    </i>
+    <i r="2">
+      <x v="23"/>
+    </i>
+    <i r="2">
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="25"/>
+    </i>
+    <i r="2">
+      <x v="26"/>
+    </i>
+    <i r="2">
+      <x v="27"/>
+    </i>
+    <i r="2">
+      <x v="28"/>
+    </i>
+    <i r="2">
+      <x v="29"/>
+    </i>
+    <i r="2">
+      <x v="30"/>
+    </i>
+    <i r="2">
+      <x v="31"/>
+    </i>
+    <i r="2">
+      <x v="32"/>
+    </i>
+    <i r="2">
+      <x v="33"/>
+    </i>
+    <i r="2">
+      <x v="34"/>
+    </i>
+    <i r="2">
+      <x v="35"/>
+    </i>
+    <i r="2">
+      <x v="36"/>
+    </i>
+    <i r="2">
+      <x v="37"/>
+    </i>
+    <i r="2">
+      <x v="38"/>
+    </i>
+    <i r="2">
+      <x v="39"/>
+    </i>
+    <i r="2">
+      <x v="40"/>
+    </i>
+    <i r="2">
+      <x v="41"/>
+    </i>
   </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField fld="10" baseField="5" baseItem="0" numFmtId="4"/>
+    <dataField fld="11" baseField="5" baseItem="0" numFmtId="3"/>
+  </dataFields>
   <pivotHierarchies count="330">
     <pivotHierarchy/>
     <pivotHierarchy/>
@@ -1427,7 +2253,7 @@
     <pivotHierarchy/>
     <pivotHierarchy/>
     <pivotHierarchy/>
-    <pivotHierarchy/>
+    <pivotHierarchy multipleItemSelectionAllowed="1"/>
     <pivotHierarchy/>
     <pivotHierarchy/>
     <pivotHierarchy/>
@@ -1667,9 +2493,13 @@
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
   </pivotHierarchies>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <rowHierarchiesUsage count="1">
+  <rowHierarchiesUsage count="2">
     <rowHierarchyUsage hierarchyUsage="120"/>
+    <rowHierarchyUsage hierarchyUsage="26"/>
   </rowHierarchiesUsage>
+  <colHierarchiesUsage count="1">
+    <colHierarchyUsage hierarchyUsage="-2"/>
+  </colHierarchiesUsage>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
@@ -1690,12 +2520,12 @@
         <level uniqueName="[TransactionDate].[YearNumber].[YearNumber]" sourceCaption="YearNumber" count="7">
           <ranges>
             <range startItem="0">
-              <i n="[TransactionDate].[YearNumber].&amp;[2011]" c="2011"/>
               <i n="[TransactionDate].[YearNumber].&amp;[2012]" c="2012"/>
               <i n="[TransactionDate].[YearNumber].&amp;[2013]" c="2013"/>
               <i n="[TransactionDate].[YearNumber].&amp;[2014]" c="2014"/>
               <i n="[TransactionDate].[YearNumber].&amp;[2015]" c="2015"/>
               <i n="[TransactionDate].[YearNumber].&amp;[2010]" c="2010" nd="1"/>
+              <i n="[TransactionDate].[YearNumber].&amp;[2011]" c="2011" nd="1"/>
               <i n="[TransactionDate].[YearNumber].&amp;" c="" nd="1"/>
             </range>
           </ranges>
@@ -1802,11 +2632,45 @@
 </slicerCacheDefinition>
 </file>
 
+<file path=xl/slicerCaches/slicerCache4.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="Slicer_PaymentUseCases" sourceName="[PaymentUseCase].[PaymentUseCases]">
+  <pivotTables>
+    <pivotTable tabId="1" name="PivotTable2"/>
+  </pivotTables>
+  <data>
+    <olap pivotCacheId="8">
+      <levels count="3">
+        <level uniqueName="[PaymentUseCase].[PaymentUseCases].[(All)]" sourceCaption="(All)" count="0"/>
+        <level uniqueName="[PaymentUseCase].[PaymentUseCases].[PaymentUseCaseType]" sourceCaption="PaymentUseCaseType" count="8">
+          <ranges>
+            <range startItem="0">
+              <i n="[PaymentUseCase].[PaymentUseCases].[PaymentUseCaseType].&amp;[Agent e-float]" c="Agent e-float"/>
+              <i n="[PaymentUseCase].[PaymentUseCases].[PaymentUseCaseType].&amp;[Cash-In | Cash-Out]" c="Cash-In | Cash-Out"/>
+              <i n="[PaymentUseCase].[PaymentUseCases].[PaymentUseCaseType].&amp;[Electronic Non-Personal Payments within MMO]" c="Electronic Non-Personal Payments within MMO"/>
+              <i n="[PaymentUseCase].[PaymentUseCases].[PaymentUseCaseType].&amp;[Electronic Payments Outgoing]" c="Electronic Payments Outgoing"/>
+              <i n="[PaymentUseCase].[PaymentUseCases].[PaymentUseCaseType].&amp;[Electronic Personal Payments within MMO]" c="Electronic Personal Payments within MMO"/>
+              <i n="[PaymentUseCase].[PaymentUseCases].[PaymentUseCaseType].&amp;[Foreign Remittances]" c="Foreign Remittances"/>
+              <i n="[PaymentUseCase].[PaymentUseCases].[PaymentUseCaseType].&amp;[Purchases from Merchant]" c="Purchases from Merchant"/>
+              <i n="[PaymentUseCase].[PaymentUseCases].[PaymentUseCaseType].&amp;[Virtual Product Payments]" c="Virtual Product Payments"/>
+            </range>
+          </ranges>
+        </level>
+        <level uniqueName="[PaymentUseCase].[PaymentUseCases].[PaymentUseCase]" sourceCaption="PaymentUseCase" count="0"/>
+      </levels>
+      <selections count="1">
+        <selection n="[PaymentUseCase].[PaymentUseCases].[PaymentUseCaseType].&amp;[Electronic Non-Personal Payments within MMO]"/>
+      </selections>
+    </olap>
+  </data>
+</slicerCacheDefinition>
+</file>
+
 <file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
 <slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
   <slicer name="YearNumber" cache="Slicer_YearNumber" caption="YearNumber" level="1" rowHeight="241300"/>
   <slicer name="MonthName" cache="Slicer_MonthName" caption="MonthName" level="1" rowHeight="241300"/>
   <slicer name="Day" cache="Slicer_Day" caption="Day" level="1" rowHeight="241300"/>
+  <slicer name="PaymentUseCaseType" cache="Slicer_PaymentUseCases" caption="PaymentUseCaseType" level="1" rowHeight="241300"/>
 </slicers>
 </file>
 
@@ -2073,38 +2937,1933 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A16:A19"/>
+  <dimension ref="A16:C189"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="4" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="67.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="4">
+        <v>354349222.76000005</v>
+      </c>
+      <c r="C17" s="5">
+        <v>23841</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="4">
+        <v>354349222.76000005</v>
+      </c>
+      <c r="C18" s="5">
+        <v>23841</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="4">
+        <v>6318321.0199999996</v>
+      </c>
+      <c r="C19" s="5">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="4">
+        <v>20710</v>
+      </c>
+      <c r="C20" s="5">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="4">
+        <v>132150</v>
+      </c>
+      <c r="C21" s="5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="4">
+        <v>157900</v>
+      </c>
+      <c r="C22" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="4">
+        <v>154.75</v>
+      </c>
+      <c r="C23" s="5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="4">
+        <v>23469061</v>
+      </c>
+      <c r="C24" s="5">
+        <v>11015</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="4">
+        <v>1216900</v>
+      </c>
+      <c r="C25" s="5">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="4">
+        <v>19739225</v>
+      </c>
+      <c r="C26" s="5">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="4">
+        <v>66000</v>
+      </c>
+      <c r="C27" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="4">
+        <v>5000</v>
+      </c>
+      <c r="C28" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="4">
+        <v>1269347.76</v>
+      </c>
+      <c r="C29" s="5">
+        <v>2834</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="4">
+        <v>2600</v>
+      </c>
+      <c r="C30" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" s="4">
+        <v>500</v>
+      </c>
+      <c r="C31" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" s="4">
+        <v>300</v>
+      </c>
+      <c r="C32" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="4">
+        <v>200</v>
+      </c>
+      <c r="C33" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="4">
+        <v>675</v>
+      </c>
+      <c r="C34" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="4">
+        <v>82000</v>
+      </c>
+      <c r="C35" s="5">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" s="4">
+        <v>486130</v>
+      </c>
+      <c r="C36" s="5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="4">
+        <v>3516620.0000000005</v>
+      </c>
+      <c r="C37" s="5">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38" s="4">
+        <v>5914</v>
+      </c>
+      <c r="C38" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B39" s="4">
+        <v>158390.5</v>
+      </c>
+      <c r="C39" s="5">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40" s="4">
+        <v>8500</v>
+      </c>
+      <c r="C40" s="5">
         <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" s="4">
+        <v>3715948.7499999995</v>
+      </c>
+      <c r="C41" s="5">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42" s="4">
+        <v>38000</v>
+      </c>
+      <c r="C42" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B43" s="4">
+        <v>3000</v>
+      </c>
+      <c r="C43" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44" s="4">
+        <v>-134000</v>
+      </c>
+      <c r="C44" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="4">
+        <v>28320902</v>
+      </c>
+      <c r="C45" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B46" s="4">
+        <v>0</v>
+      </c>
+      <c r="C46" s="5">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B47" s="4">
+        <v>8147280.6299999999</v>
+      </c>
+      <c r="C47" s="5">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B48" s="4">
+        <v>70028026</v>
+      </c>
+      <c r="C48" s="5">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49" s="4">
+        <v>0</v>
+      </c>
+      <c r="C49" s="5">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B50" s="4">
+        <v>29592301.240000002</v>
+      </c>
+      <c r="C50" s="5">
+        <v>1659</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B51" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="C51" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B52" s="4">
+        <v>80024026</v>
+      </c>
+      <c r="C52" s="5">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B53" s="4">
+        <v>-195850</v>
+      </c>
+      <c r="C53" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B54" s="4">
+        <v>61331100</v>
+      </c>
+      <c r="C54" s="5">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B55" s="4">
+        <v>741370</v>
+      </c>
+      <c r="C55" s="5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B56" s="4">
+        <v>4991098</v>
+      </c>
+      <c r="C56" s="5">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B57" s="4">
+        <v>21</v>
+      </c>
+      <c r="C57" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B58" s="4">
+        <v>36015.15</v>
+      </c>
+      <c r="C58" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B59" s="4">
+        <v>1053384.96</v>
+      </c>
+      <c r="C59" s="5">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B60" s="4">
+        <v>0</v>
+      </c>
+      <c r="C60" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" s="4">
+        <v>354349222.76000005</v>
+      </c>
+      <c r="C61" s="5">
+        <v>23841</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B62" s="4">
+        <v>6318321.0199999996</v>
+      </c>
+      <c r="C62" s="5">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B63" s="4">
+        <v>20710</v>
+      </c>
+      <c r="C63" s="5">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B64" s="4">
+        <v>132150</v>
+      </c>
+      <c r="C64" s="5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B65" s="4">
+        <v>157900</v>
+      </c>
+      <c r="C65" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B66" s="4">
+        <v>154.75</v>
+      </c>
+      <c r="C66" s="5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B67" s="4">
+        <v>23469061</v>
+      </c>
+      <c r="C67" s="5">
+        <v>11015</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B68" s="4">
+        <v>1216900</v>
+      </c>
+      <c r="C68" s="5">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B69" s="4">
+        <v>19739225</v>
+      </c>
+      <c r="C69" s="5">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B70" s="4">
+        <v>66000</v>
+      </c>
+      <c r="C70" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B71" s="4">
+        <v>5000</v>
+      </c>
+      <c r="C71" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B72" s="4">
+        <v>1269347.76</v>
+      </c>
+      <c r="C72" s="5">
+        <v>2834</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B73" s="4">
+        <v>2600</v>
+      </c>
+      <c r="C73" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B74" s="4">
+        <v>500</v>
+      </c>
+      <c r="C74" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B75" s="4">
+        <v>300</v>
+      </c>
+      <c r="C75" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B76" s="4">
+        <v>200</v>
+      </c>
+      <c r="C76" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B77" s="4">
+        <v>675</v>
+      </c>
+      <c r="C77" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B78" s="4">
+        <v>82000</v>
+      </c>
+      <c r="C78" s="5">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B79" s="4">
+        <v>486130</v>
+      </c>
+      <c r="C79" s="5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B80" s="4">
+        <v>3516620.0000000005</v>
+      </c>
+      <c r="C80" s="5">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B81" s="4">
+        <v>5914</v>
+      </c>
+      <c r="C81" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B82" s="4">
+        <v>158390.5</v>
+      </c>
+      <c r="C82" s="5">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B83" s="4">
+        <v>8500</v>
+      </c>
+      <c r="C83" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B84" s="4">
+        <v>3715948.7499999995</v>
+      </c>
+      <c r="C84" s="5">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B85" s="4">
+        <v>38000</v>
+      </c>
+      <c r="C85" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B86" s="4">
+        <v>3000</v>
+      </c>
+      <c r="C86" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B87" s="4">
+        <v>-134000</v>
+      </c>
+      <c r="C87" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B88" s="4">
+        <v>28320902</v>
+      </c>
+      <c r="C88" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B89" s="4">
+        <v>0</v>
+      </c>
+      <c r="C89" s="5">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B90" s="4">
+        <v>8147280.6299999999</v>
+      </c>
+      <c r="C90" s="5">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B91" s="4">
+        <v>70028026</v>
+      </c>
+      <c r="C91" s="5">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B92" s="4">
+        <v>0</v>
+      </c>
+      <c r="C92" s="5">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B93" s="4">
+        <v>29592301.240000002</v>
+      </c>
+      <c r="C93" s="5">
+        <v>1659</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B94" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="C94" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B95" s="4">
+        <v>80024026</v>
+      </c>
+      <c r="C95" s="5">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B96" s="4">
+        <v>-195850</v>
+      </c>
+      <c r="C96" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B97" s="4">
+        <v>61331100</v>
+      </c>
+      <c r="C97" s="5">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B98" s="4">
+        <v>741370</v>
+      </c>
+      <c r="C98" s="5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B99" s="4">
+        <v>4991098</v>
+      </c>
+      <c r="C99" s="5">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B100" s="4">
+        <v>21</v>
+      </c>
+      <c r="C100" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B101" s="4">
+        <v>36015.15</v>
+      </c>
+      <c r="C101" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B102" s="4">
+        <v>1053384.96</v>
+      </c>
+      <c r="C102" s="5">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B103" s="4">
+        <v>0</v>
+      </c>
+      <c r="C103" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B104" s="4">
+        <v>354349222.76000005</v>
+      </c>
+      <c r="C104" s="5">
+        <v>23841</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B105" s="4">
+        <v>6318321.0199999996</v>
+      </c>
+      <c r="C105" s="5">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B106" s="4">
+        <v>20710</v>
+      </c>
+      <c r="C106" s="5">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B107" s="4">
+        <v>132150</v>
+      </c>
+      <c r="C107" s="5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B108" s="4">
+        <v>157900</v>
+      </c>
+      <c r="C108" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B109" s="4">
+        <v>154.75</v>
+      </c>
+      <c r="C109" s="5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B110" s="4">
+        <v>23469061</v>
+      </c>
+      <c r="C110" s="5">
+        <v>11015</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B111" s="4">
+        <v>1216900</v>
+      </c>
+      <c r="C111" s="5">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B112" s="4">
+        <v>19739225</v>
+      </c>
+      <c r="C112" s="5">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B113" s="4">
+        <v>66000</v>
+      </c>
+      <c r="C113" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B114" s="4">
+        <v>5000</v>
+      </c>
+      <c r="C114" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B115" s="4">
+        <v>1269347.76</v>
+      </c>
+      <c r="C115" s="5">
+        <v>2834</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B116" s="4">
+        <v>2600</v>
+      </c>
+      <c r="C116" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B117" s="4">
+        <v>500</v>
+      </c>
+      <c r="C117" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B118" s="4">
+        <v>300</v>
+      </c>
+      <c r="C118" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B119" s="4">
+        <v>200</v>
+      </c>
+      <c r="C119" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B120" s="4">
+        <v>675</v>
+      </c>
+      <c r="C120" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B121" s="4">
+        <v>82000</v>
+      </c>
+      <c r="C121" s="5">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B122" s="4">
+        <v>486130</v>
+      </c>
+      <c r="C122" s="5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B123" s="4">
+        <v>3516620.0000000005</v>
+      </c>
+      <c r="C123" s="5">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B124" s="4">
+        <v>5914</v>
+      </c>
+      <c r="C124" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B125" s="4">
+        <v>158390.5</v>
+      </c>
+      <c r="C125" s="5">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B126" s="4">
+        <v>8500</v>
+      </c>
+      <c r="C126" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B127" s="4">
+        <v>3715948.7499999995</v>
+      </c>
+      <c r="C127" s="5">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B128" s="4">
+        <v>38000</v>
+      </c>
+      <c r="C128" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B129" s="4">
+        <v>3000</v>
+      </c>
+      <c r="C129" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B130" s="4">
+        <v>-134000</v>
+      </c>
+      <c r="C130" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B131" s="4">
+        <v>28320902</v>
+      </c>
+      <c r="C131" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B132" s="4">
+        <v>0</v>
+      </c>
+      <c r="C132" s="5">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B133" s="4">
+        <v>8147280.6299999999</v>
+      </c>
+      <c r="C133" s="5">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B134" s="4">
+        <v>70028026</v>
+      </c>
+      <c r="C134" s="5">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B135" s="4">
+        <v>0</v>
+      </c>
+      <c r="C135" s="5">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B136" s="4">
+        <v>29592301.240000002</v>
+      </c>
+      <c r="C136" s="5">
+        <v>1659</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B137" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="C137" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B138" s="4">
+        <v>80024026</v>
+      </c>
+      <c r="C138" s="5">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B139" s="4">
+        <v>-195850</v>
+      </c>
+      <c r="C139" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B140" s="4">
+        <v>61331100</v>
+      </c>
+      <c r="C140" s="5">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B141" s="4">
+        <v>741370</v>
+      </c>
+      <c r="C141" s="5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B142" s="4">
+        <v>4991098</v>
+      </c>
+      <c r="C142" s="5">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B143" s="4">
+        <v>21</v>
+      </c>
+      <c r="C143" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B144" s="4">
+        <v>36015.15</v>
+      </c>
+      <c r="C144" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B145" s="4">
+        <v>1053384.96</v>
+      </c>
+      <c r="C145" s="5">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B146" s="4">
+        <v>0</v>
+      </c>
+      <c r="C146" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B147" s="4">
+        <v>354349222.76000005</v>
+      </c>
+      <c r="C147" s="5">
+        <v>23841</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B148" s="4">
+        <v>6318321.0199999996</v>
+      </c>
+      <c r="C148" s="5">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B149" s="4">
+        <v>20710</v>
+      </c>
+      <c r="C149" s="5">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B150" s="4">
+        <v>132150</v>
+      </c>
+      <c r="C150" s="5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B151" s="4">
+        <v>157900</v>
+      </c>
+      <c r="C151" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B152" s="4">
+        <v>154.75</v>
+      </c>
+      <c r="C152" s="5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B153" s="4">
+        <v>23469061</v>
+      </c>
+      <c r="C153" s="5">
+        <v>11015</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B154" s="4">
+        <v>1216900</v>
+      </c>
+      <c r="C154" s="5">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B155" s="4">
+        <v>19739225</v>
+      </c>
+      <c r="C155" s="5">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B156" s="4">
+        <v>66000</v>
+      </c>
+      <c r="C156" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B157" s="4">
+        <v>5000</v>
+      </c>
+      <c r="C157" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B158" s="4">
+        <v>1269347.76</v>
+      </c>
+      <c r="C158" s="5">
+        <v>2834</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B159" s="4">
+        <v>2600</v>
+      </c>
+      <c r="C159" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B160" s="4">
+        <v>500</v>
+      </c>
+      <c r="C160" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B161" s="4">
+        <v>300</v>
+      </c>
+      <c r="C161" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B162" s="4">
+        <v>200</v>
+      </c>
+      <c r="C162" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B163" s="4">
+        <v>675</v>
+      </c>
+      <c r="C163" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B164" s="4">
+        <v>82000</v>
+      </c>
+      <c r="C164" s="5">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B165" s="4">
+        <v>486130</v>
+      </c>
+      <c r="C165" s="5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B166" s="4">
+        <v>3516620.0000000005</v>
+      </c>
+      <c r="C166" s="5">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B167" s="4">
+        <v>5914</v>
+      </c>
+      <c r="C167" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B168" s="4">
+        <v>158390.5</v>
+      </c>
+      <c r="C168" s="5">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B169" s="4">
+        <v>8500</v>
+      </c>
+      <c r="C169" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B170" s="4">
+        <v>3715948.7499999995</v>
+      </c>
+      <c r="C170" s="5">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B171" s="4">
+        <v>38000</v>
+      </c>
+      <c r="C171" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B172" s="4">
+        <v>3000</v>
+      </c>
+      <c r="C172" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B173" s="4">
+        <v>-134000</v>
+      </c>
+      <c r="C173" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B174" s="4">
+        <v>28320902</v>
+      </c>
+      <c r="C174" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B175" s="4">
+        <v>0</v>
+      </c>
+      <c r="C175" s="5">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B176" s="4">
+        <v>8147280.6299999999</v>
+      </c>
+      <c r="C176" s="5">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B177" s="4">
+        <v>70028026</v>
+      </c>
+      <c r="C177" s="5">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B178" s="4">
+        <v>0</v>
+      </c>
+      <c r="C178" s="5">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B179" s="4">
+        <v>29592301.240000002</v>
+      </c>
+      <c r="C179" s="5">
+        <v>1659</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B180" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="C180" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B181" s="4">
+        <v>80024026</v>
+      </c>
+      <c r="C181" s="5">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B182" s="4">
+        <v>-195850</v>
+      </c>
+      <c r="C182" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B183" s="4">
+        <v>61331100</v>
+      </c>
+      <c r="C183" s="5">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B184" s="4">
+        <v>741370</v>
+      </c>
+      <c r="C184" s="5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B185" s="4">
+        <v>4991098</v>
+      </c>
+      <c r="C185" s="5">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B186" s="4">
+        <v>21</v>
+      </c>
+      <c r="C186" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B187" s="4">
+        <v>36015.15</v>
+      </c>
+      <c r="C187" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B188" s="4">
+        <v>1053384.96</v>
+      </c>
+      <c r="C188" s="5">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B189" s="4">
+        <v>0</v>
+      </c>
+      <c r="C189" s="5">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>